<commit_message>
Subindo modelo fisico atualizado e criação dos scripts
</commit_message>
<xml_diff>
--- a/bd/MER/ModelagemBD/ModelagemFisica.xlsx
+++ b/bd/MER/ModelagemBD/ModelagemFisica.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fic\Desktop\Projeto_ProVagas\bd\MER\ModelagemBD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Projeto_ProVagas\bd\MER\ModelagemBD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474C10FF-EC62-42DD-B8B8-582F8B56B44D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9211BB4-D40F-4395-842B-9329DF5057A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{49616955-74A9-4DCD-839A-5AC96D81C1FF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="125">
   <si>
     <t>TipoUsuario</t>
   </si>
@@ -105,9 +105,6 @@
     <t>IdTipoVaga</t>
   </si>
   <si>
-    <t>DataInscricao</t>
-  </si>
-  <si>
     <t>IdStatusInscricao</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>CEP</t>
   </si>
   <si>
-    <t>311-31-312</t>
-  </si>
-  <si>
     <t>b@email.com</t>
   </si>
   <si>
@@ -243,15 +237,6 @@
     <t>99999-9999</t>
   </si>
   <si>
-    <t>123-54-342</t>
-  </si>
-  <si>
-    <t>321-23-345</t>
-  </si>
-  <si>
-    <t>214-64-345</t>
-  </si>
-  <si>
     <t>Beneficio</t>
   </si>
   <si>
@@ -373,6 +358,48 @@
   </si>
   <si>
     <t>Estagio</t>
+  </si>
+  <si>
+    <t>DataNascimento</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>Pedro da Silva</t>
+  </si>
+  <si>
+    <t>Bruno Oliveira</t>
+  </si>
+  <si>
+    <t>NomeCompletoCandidato</t>
+  </si>
+  <si>
+    <t>IdAdministrador</t>
+  </si>
+  <si>
+    <t>NomeCompletoAdmin</t>
+  </si>
+  <si>
+    <t>Roberto Pereirea</t>
+  </si>
+  <si>
+    <t>Priscila Mattos</t>
+  </si>
+  <si>
+    <t>31131-312</t>
+  </si>
+  <si>
+    <t>12354-342</t>
+  </si>
+  <si>
+    <t>32123-345</t>
+  </si>
+  <si>
+    <t>21494-345</t>
+  </si>
+  <si>
+    <t>xxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -396,7 +423,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,12 +468,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCC00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -519,12 +540,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -532,6 +547,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -558,39 +579,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -608,17 +635,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -945,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08154577-7DCB-4B1D-81C7-57F28EF0A2C9}">
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,31 +986,32 @@
     <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
     <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="9" max="9" width="38.7109375" customWidth="1"/>
     <col min="10" max="10" width="24.85546875" customWidth="1"/>
     <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" customWidth="1"/>
     <col min="17" max="17" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="27"/>
+      <c r="D1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="G1" s="25" t="s">
+      <c r="E1" s="23"/>
+      <c r="G1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -998,25 +1024,25 @@
         <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="K2" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>12</v>
@@ -1033,28 +1059,28 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="M3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1068,28 +1094,28 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" s="4">
         <v>2</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="M4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1103,7 +1129,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1111,24 +1137,24 @@
         <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
+      <c r="A8" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="34"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
@@ -1143,31 +1169,28 @@
         <v>18</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="I9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1175,36 +1198,33 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="5">
         <v>231</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="J10" s="5">
         <v>1</v>
       </c>
       <c r="K10" s="5">
-        <v>1</v>
-      </c>
-      <c r="L10" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1213,36 +1233,33 @@
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="5">
         <v>341</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="J11" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K11" s="5">
-        <v>2</v>
-      </c>
-      <c r="L11" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1251,36 +1268,33 @@
         <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12" s="5">
         <v>234</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="I12" s="5" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="J12" s="5">
         <v>3</v>
       </c>
       <c r="K12" s="5">
-        <v>3</v>
-      </c>
-      <c r="L12" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1289,51 +1303,48 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E13" s="5">
         <v>543</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="J13" s="5">
         <v>4</v>
       </c>
       <c r="K13" s="5">
-        <v>4</v>
-      </c>
-      <c r="L13" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
+      <c r="A15" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="34"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -1360,28 +1371,26 @@
       <c r="H16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="I16" s="33"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>1</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" s="7">
         <v>1</v>
@@ -1389,85 +1398,81 @@
       <c r="H17" s="7">
         <v>1</v>
       </c>
-      <c r="I17" s="7">
-        <v>1</v>
-      </c>
+      <c r="I17" s="33"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>2</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="7">
+        <v>2</v>
+      </c>
+      <c r="H18" s="7">
+        <v>2</v>
+      </c>
+      <c r="I18" s="33"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="D21" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="G21" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" s="26"/>
+      <c r="J21" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="7">
-        <v>2</v>
-      </c>
-      <c r="H18" s="7">
-        <v>2</v>
-      </c>
-      <c r="I18" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="24"/>
-      <c r="D21" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="21"/>
-      <c r="G21" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" s="22"/>
-      <c r="J21" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="K22" s="11" t="s">
         <v>24</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1475,19 +1480,19 @@
         <v>1</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="9">
         <v>1</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G23" s="10">
         <v>1</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J23" s="11">
         <v>1</v>
@@ -1504,19 +1509,19 @@
         <v>2</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="9">
         <v>2</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G24" s="10">
         <v>2</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="J24" s="11">
         <v>2</v>
@@ -1533,19 +1538,19 @@
         <v>3</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="9">
         <v>3</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G25" s="10">
         <v>3</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J25" s="11">
         <v>3</v>
@@ -1562,13 +1567,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G26" s="10">
         <v>4</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J26" s="11">
         <v>4</v>
@@ -1585,7 +1590,7 @@
         <v>5</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J27" s="11">
         <v>5</v>
@@ -1598,47 +1603,35 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
       <c r="G28" s="10">
         <v>6</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
       <c r="G29" s="10">
         <v>7</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
       <c r="G30" s="10">
         <v>8</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
       <c r="G31" s="10">
         <v>9</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1646,168 +1639,294 @@
         <v>10</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="D34" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1</v>
+      </c>
+      <c r="H35" s="16"/>
+      <c r="I35" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="J35" s="19"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
+        <v>2</v>
+      </c>
+      <c r="B36" s="5">
+        <v>2</v>
+      </c>
+      <c r="C36" s="5">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5">
+        <v>2</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="K36" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="L36" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H37" s="17">
+        <v>1</v>
+      </c>
+      <c r="I37" s="18">
+        <v>44078</v>
+      </c>
+      <c r="J37" s="18">
+        <v>44869</v>
+      </c>
+      <c r="K37" s="17">
+        <v>1</v>
+      </c>
+      <c r="L37" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="E38" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="22"/>
+      <c r="H38" s="17">
+        <v>2</v>
+      </c>
+      <c r="I38" s="18">
+        <v>44079</v>
+      </c>
+      <c r="J38" s="18">
+        <v>44899</v>
+      </c>
+      <c r="K38" s="17">
+        <v>2</v>
+      </c>
+      <c r="L38" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <v>1</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="13">
+        <v>1</v>
+      </c>
+      <c r="E40" s="14">
+        <v>1</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>2</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="13">
+        <v>2</v>
+      </c>
+      <c r="E41" s="14">
+        <v>2</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H41" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H42" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H43" s="5">
+        <v>1</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J43" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="H44" s="5">
+        <v>2</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J44" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>1</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="5">
-        <v>1</v>
-      </c>
-      <c r="D35" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
-        <v>2</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="5">
-        <v>2</v>
-      </c>
-      <c r="D36" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="E38" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="F38" s="18"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
-        <v>1</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="14">
-        <v>1</v>
-      </c>
-      <c r="E40" s="15">
-        <v>1</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="14">
-        <v>2</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C41" s="14">
-        <v>2</v>
-      </c>
-      <c r="E41" s="15">
-        <v>2</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="29"/>
-      <c r="C45" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="28" t="s">
+      <c r="D45" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>1</v>
+      </c>
+      <c r="B46" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="C46" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="28" t="s">
+      <c r="C46" s="32">
+        <v>44808</v>
+      </c>
+      <c r="D46" s="4">
+        <v>32143565432</v>
+      </c>
+      <c r="E46" s="4">
+        <v>2</v>
+      </c>
+      <c r="F46" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>2</v>
+      </c>
+      <c r="B47" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="E46" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="31">
-        <v>1</v>
-      </c>
       <c r="C47" s="32">
-        <v>44078</v>
-      </c>
-      <c r="D47" s="32">
         <v>44808</v>
       </c>
-      <c r="E47" s="31">
-        <v>1</v>
-      </c>
-      <c r="F47" s="31">
-        <v>2</v>
-      </c>
+      <c r="D47" s="4">
+        <v>32454745434</v>
+      </c>
+      <c r="E47" s="4">
+        <v>4</v>
+      </c>
+      <c r="F47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F48" s="33"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="A8:L8"/>
+  <mergeCells count="15">
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="I35:J35"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="D1:E1"/>
@@ -1817,7 +1936,6 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="G1:M1"/>
-    <mergeCell ref="A15:I15"/>
     <mergeCell ref="A33:D33"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>